<commit_message>
dev responses to the Referees of Chaos
</commit_message>
<xml_diff>
--- a/doc/runtimes_0.1s.xlsx
+++ b/doc/runtimes_0.1s.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothytyree/Documents/GitHub/bgmc/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B805A9-973D-D54A-A47C-2670FF3DFD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C420F499-68E2-1146-BC63-5F03FF4EF307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2240" windowWidth="27580" windowHeight="17440" xr2:uid="{FA1833FB-E3E1-E34C-A061-C957393A5EA4}"/>
+    <workbookView xWindow="0" yWindow="2240" windowWidth="27580" windowHeight="17440" activeTab="1" xr2:uid="{FA1833FB-E3E1-E34C-A061-C957393A5EA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
   <si>
     <t>model</t>
   </si>
@@ -55,6 +56,9 @@
   </si>
   <si>
     <t>pct_speedup (%)</t>
+  </si>
+  <si>
+    <t>simtime (s)</t>
   </si>
 </sst>
 </file>
@@ -428,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8673A30B-5E5E-9044-A594-F31D58183A4B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="47" x14ac:dyDescent="0.55000000000000004"/>
@@ -484,6 +488,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DB03FB-8A68-4A4B-A12B-8BAB7DFDC0F8}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="47" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>127</v>
+      </c>
+      <c r="D2">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="E2">
+        <f>(C2-D2)/D2*100</f>
+        <v>12780.324543610546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>31.4</v>
+      </c>
+      <c r="D3">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="E3">
+        <f>(C3-D3)/D3*100</f>
+        <v>26286.55462184874</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B3B31A-64D1-E447-8BD6-98CCC776FA6B}">
   <dimension ref="A1:D3"/>
   <sheetViews>

</xml_diff>